<commit_message>
Manual Testcases added to buyerhub
</commit_message>
<xml_diff>
--- a/Buyer hub/Invoices/Automated testcases/Invoice listing final testcases.xlsx
+++ b/Buyer hub/Invoices/Automated testcases/Invoice listing final testcases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testcases one group\Buyer hub\Invoices\Manual testcases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Zeemart All\Git hub\zm-buyerautomation\Buyer hub\Invoices\Automated testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33310103-15CC-4C88-97E3-66E268ABD854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AE7EAC-49CB-459C-8AE2-C3858708BF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2758FE1B-EF22-4ECC-8673-3C2C9DDE616F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="72">
   <si>
     <t>SL. No</t>
   </si>
@@ -340,12 +340,30 @@
   <si>
     <t>It get displayed Invoice processed details and underline in blue colour</t>
   </si>
+  <si>
+    <t>In Invoices, non-ZM suppliers appear in the “Supplier” filter</t>
+  </si>
+  <si>
+    <t>In Invoice details, the invoice details contains the same options like a normal e-invoice, but there may or may not be an order listed under “Linked to”. If there is an order, it will not be hyperlinked</t>
+  </si>
+  <si>
+    <t>As expected it displayed the  same options like a normal e-invoice, but there may or may not be an order listed under “Linked to”. If there is an order, it will not be hyperlinked</t>
+  </si>
+  <si>
+    <t>Click the Invoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Non-ZM suppliers should appear in the Xero/QBO integration settings page, to allow for “supplier mapping”.</t>
+  </si>
+  <si>
+    <t>As expected it allowed supplier mapping</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,12 +394,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -397,7 +409,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -420,35 +432,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -460,27 +448,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105319C2-CA92-4291-B439-CA8F566CD853}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,6 +795,7 @@
     <col min="5" max="5" width="60.28515625" customWidth="1"/>
     <col min="6" max="6" width="51.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -887,22 +873,22 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -968,13 +954,13 @@
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="10" t="s">
         <v>38</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -992,13 +978,13 @@
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="10" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -1007,7 +993,7 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1016,21 +1002,22 @@
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1039,21 +1026,22 @@
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="10" t="s">
         <v>50</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1062,21 +1050,22 @@
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="10" t="s">
         <v>51</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1085,21 +1074,22 @@
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="10" t="s">
         <v>50</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1108,21 +1098,22 @@
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="10" t="s">
         <v>56</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1131,180 +1122,240 @@
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="10" t="s">
         <v>50</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="G15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="9">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="G16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="G17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="9" t="s">
+      <c r="G18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="2"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="9"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="9"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="9"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
     </row>
   </sheetData>
@@ -1314,6 +1365,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE14CF829741B9429012C5963B61706A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18d29298087f70c59de6e7c2ad40e873">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="014d4624-f59d-44c3-a333-b6c591c77b53" xmlns:ns4="7c8c12dd-75f8-42a3-90db-eecf595a7e04" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="150812ec1dd04a19c671e952e2c5ff5b" ns3:_="" ns4:_="">
     <xsd:import namespace="014d4624-f59d-44c3-a333-b6c591c77b53"/>
@@ -1516,15 +1576,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1532,6 +1583,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13421BFF-B42C-4D11-87F9-0ABC088A76EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{534C194C-7EE7-400B-A072-57A88857D538}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1546,14 +1605,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13421BFF-B42C-4D11-87F9-0ABC088A76EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>